<commit_message>
221024 biosyn, need update sp!
</commit_message>
<xml_diff>
--- a/source_plates/221024_arpae_plasmids.xlsx
+++ b/source_plates/221024_arpae_plasmids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\WHISPR\source_plates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D2DAD1-7A62-439D-8C14-B1E81FF7D765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D3CBE-4C2F-4412-82F3-DE378729F754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>